<commit_message>
added viewing the existing calibration models
</commit_message>
<xml_diff>
--- a/DataDashboard/webapp/lysate_data_import/Calibration/data/GFP_uM_Polynomial_Sarah_Oct_22.xlsx
+++ b/DataDashboard/webapp/lysate_data_import/Calibration/data/GFP_uM_Polynomial_Sarah_Oct_22.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_6F8E825FCBA2EA1C1248B86B66BD64D41E0CA8D0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F124ABB7-0540-475D-AA53-0D713AF871E2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="-23280" yWindow="3480" windowWidth="21540" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,22 +20,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Concentration (uM)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="7">
   <si>
     <t>RFU</t>
+  </si>
+  <si>
+    <t>Synergy H1_22060313</t>
+  </si>
+  <si>
+    <t>Plate_Reader</t>
+  </si>
+  <si>
+    <t>Gain</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>GFP</t>
+  </si>
+  <si>
+    <t>Concentration_uM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,6 +102,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -344,76 +370,139 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.453125" customWidth="1"/>
-    <col min="2" max="2" width="17.36328125" customWidth="1"/>
+    <col min="1" max="2" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>0</v>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
         <v>0.15</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>98.666666666666657</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
         <v>0.3</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>245</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
         <v>0.6</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>682</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>1.17</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>1925.3333333333333</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>4128</v>
       </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>